<commit_message>
Biotech Expansion - Insectoid 글자 깨짐 수정
</commit_message>
<xml_diff>
--- a/Data/Biotech Expansion - Insectoid - 3219625470/Biotech Expansion - Insectoid - 3219625470.xlsx
+++ b/Data/Biotech Expansion - Insectoid - 3219625470/Biotech Expansion - Insectoid - 3219625470.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zilrt\Desktop\Biotech Expansion - Insectoid - 3219625470\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\Biotech Expansion - Insectoid - 3219625470\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6B1BE5-02E0-4529-AC16-A92854215C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03EBF03-9CFC-4BF9-B8FE-B929D8E78F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-3760" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>food to jelly transmutation (OBSOLETE)</t>
   </si>
   <si>
-    <t>음식을 젤리로 변성(쓸모없음)</t>
-  </si>
-  <si>
     <t>AbilityDef+BTEIst_JellyTransmutation.description</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Convert some food in the world into precious insect jelly. Wastes a considerable amount of nutrition (20%). This is an old version of the ability for save compatibility purposes. Please reload the pawn's xenotype for the newer version. (Using this ability again when the pawn has the newer ability will delete this one.)</t>
   </si>
   <si>
-    <t>음식을 귀중한 곤충젤리로 변성합니다. 상당한 양(20%)의 영양분이 낭비됩니다. 이것은 호환성 목적을 위해 남겨둔 구버전입니다. 폰의 인종형을 새 버전으로 재로드해주십시오. (폰에게 신버전의 능력이 있을 경우 이 능력을 다시 사용하면 이 능력은 사라집니다.)</t>
-  </si>
-  <si>
     <t>AbilityDef+BTEIst_JellyTransmutationer.label</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>food to jelly transmutation</t>
   </si>
   <si>
-    <t>음식을 젤리로 변성</t>
-  </si>
-  <si>
     <t>AbilityDef+BTEIst_JellyTransmutationer.description</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
   </si>
   <si>
     <t>Convert some food in the world into precious insect jelly. Wastes a considerable amount of nutrition (20%).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">음식을 귀중한 곤충젤리로 변성합니다. 상당한 양(20%)의 영양분이 낭비됩니다. </t>
   </si>
   <si>
     <t>AbilityDef+BTEIst_ToxInject.label</t>
@@ -1786,6 +1774,22 @@
   </si>
   <si>
     <t>스플라이스-스케럽들은 개조둥지의 노동자 계급이며, 긴 시간동안 일할 수 있고, 날음식을 곤충젤리로 전환하는 능력을 지니고 있습니다.</t>
+  </si>
+  <si>
+    <t>음식을 젤리로 변성(쓸모없음)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>음식을 귀중한 곤충젤리로 변성합니다. 상당한 양(20%)의 영양분이 낭비됩니다. 이것은 호환성 목적을 위해 남겨둔 구버전입니다. 폰의 인종형을 새 버전으로 재로드해주십시오. (폰에게 신버전의 능력이 있을 경우 이 능력을 다시 사용하면 이 능력은 사라집니다.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>음식을 젤리로 변성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>음식을 귀중한 곤충젤리로 변성합니다. 상당한 양(20%)의 영양분이 낭비됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1834,7 +1838,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2139,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2254,1035 +2258,1035 @@
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>579</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>580</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>34</v>
+        <v>581</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>582</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
@@ -3296,1464 +3300,1464 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="F141" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="F145" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>